<commit_message>
fix(lib): update the cloud sovereignty framework to v1.2.1 (#2795)
* fix(lib): update the cloud sovereignty framework to v1.2.1

* add excel sheet

* update readme
</commit_message>
<xml_diff>
--- a/tools/excel/EU/cloud-sovereignty-framework.xlsx
+++ b/tools/excel/EU/cloud-sovereignty-framework.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abder/mydev/intuitem/staging/ciso-assistant-community/tools/excel/EU/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DE6557-5301-DE49-B38E-30443BB778EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A8890D7-047D-504F-B329-D038B5DD10A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4020" yWindow="-28020" windowWidth="50880" windowHeight="27860" activeTab="2" xr2:uid="{C1B9C957-850F-8443-8E06-CB4E729FFF6E}"/>
   </bookViews>
@@ -161,9 +161,6 @@
     <t>urn:intuitem:risk:library:cloud-sovereignty-framework</t>
   </si>
   <si>
-    <t>Cloud Sovereignty Framework - version 1.2 - Sep 2025</t>
-  </si>
-  <si>
     <t>EUROPEAN COMMISSION</t>
   </si>
   <si>
@@ -242,12 +239,6 @@
 resilience against external dependencies.</t>
   </si>
   <si>
-    <t>Supply chain sovereignty evaluates the geographic origin,
-transparency, and resilience of the technology supply chain, focusing
-on the extent to which critical components and processes remain under
-EU control or exposed to non-EU dependencies.</t>
-  </si>
-  <si>
     <t>Technology sovereignty evaluates the degree of openness,
 transparency, and independence in the underlying technological
 stack, ensuring EU actors can interoperate, audit, and evolve solutions
@@ -258,11 +249,6 @@
 security operations, compliance obligations, and resilience measures
 are controlled within the EU, ensuring independence from foreign
 jurisdictions and long-term operational assurance.</t>
-  </si>
-  <si>
-    <t>Environmental sustainability assesses autonomy and resilience of cloud
-services over the long term in relation to energy usage, dependency and
-raw material scarcity.</t>
   </si>
   <si>
     <t>- Ensuring that bodies having decisive authority over your services are located within EU jurisdiction,
@@ -310,19 +296,29 @@
 - Degree of EU independence in high-performance computing capabilities, including processors, accelerators, and software ecosystems.</t>
   </si>
   <si>
-    <t>- Attainment of EU and internationally recognized certifications (e.g.,
-ISO, ENISA schemes)
+    <t>- Adoption of energy-efficient infrastructure (e.g., low PUE) and measurable improvement targets.
+- Circular economy practices ensuring reuse, refurbishment, and responsible end-of-life treatment of hardware.
+- Transparent measurement and disclosure of carbon emissions, water usage, and other sustainability indicators.
+- Sourcing of renewable or low-carbon energy to power infrastructure and operations</t>
+  </si>
+  <si>
+    <t>Cloud Sovereignty Framework - version 1.2.1 - Oct 2025</t>
+  </si>
+  <si>
+    <t>Supply chain sovereignty evaluates the geographic origin,
+transparency, and resilience of the technology supply chain, focusing
+on the extent to which critical components and processes remain under EU control or exposed to non-EU dependencies.</t>
+  </si>
+  <si>
+    <t>Environmental sustainability assesses autonomy and resilience of cloud services over the long term in relation to energy usage, dependency and raw material scarcity.</t>
+  </si>
+  <si>
+    <t>- Attainment of EU and internationally recognized certifications (e.g., ISO, ENISA schemes)
 - Adherence to GDPR, NIS2, DORA, and other EU frameworks
 - Security Operations Centres and response teams operating
 exclusively under EU jurisdiction, control over security monitoring/logging - customer or EU authority ability to oversee logs, alerts, and monitoring functions directly.
 - Transparent, timely, and EU-compliant reporting of breaches or vulnerabilities, maintenance Autonomy - ability to develop, test, and apply security patches independently of non-EU vendors
 - Capacity for EU entities to perform independent security and compliance audits with full access.</t>
-  </si>
-  <si>
-    <t>- Adoption of energy-efficient infrastructure (e.g., low PUE) and measurable improvement targets.
-- Circular economy practices ensuring reuse, refurbishment, and responsible end-of-life treatment of hardware.
-- Transparent measurement and disclosure of carbon emissions, water usage, and other sustainability indicators.
-- Sourcing of renewable or low-carbon energy to power infrastructure and operations</t>
   </si>
 </sst>
 </file>
@@ -720,7 +716,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView zoomScale="263" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -751,7 +747,7 @@
         <v>20</v>
       </c>
       <c r="B3" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -759,7 +755,7 @@
         <v>21</v>
       </c>
       <c r="B4" s="3">
-        <v>45930</v>
+        <v>45960</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
@@ -791,7 +787,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -799,7 +795,7 @@
         <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -807,7 +803,7 @@
         <v>25</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -820,6 +816,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -828,7 +825,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="186" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4:B6"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -883,7 +880,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>38</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -920,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{849FBD4A-EA94-AF41-9BE9-A360FB46E498}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="206" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="206" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -948,30 +945,30 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
         <v>56</v>
-      </c>
-      <c r="G1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G2">
         <v>15</v>
@@ -979,22 +976,22 @@
     </row>
     <row r="3" spans="1:7" ht="136" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G3">
         <v>10</v>
@@ -1002,22 +999,22 @@
     </row>
     <row r="4" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="G4">
         <v>10</v>
@@ -1025,45 +1022,45 @@
     </row>
     <row r="5" spans="1:7" ht="204" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G5">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="G6">
         <v>20</v>
@@ -1071,22 +1068,22 @@
     </row>
     <row r="7" spans="1:7" ht="153" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G7">
         <v>15</v>
@@ -1094,22 +1091,22 @@
     </row>
     <row r="8" spans="1:7" ht="187" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="G8">
         <v>10</v>
@@ -1117,22 +1114,22 @@
     </row>
     <row r="9" spans="1:7" ht="119" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G9">
         <v>5</v>
@@ -1180,7 +1177,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A78255AD-6FD9-F441-8C48-7096C47B1FCA}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="200" workbookViewId="0">
       <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>

</xml_diff>